<commit_message>
Fixed shell bug, removed duplicate C12 line
</commit_message>
<xml_diff>
--- a/Nuclear Materials Datasheet.xlsx
+++ b/Nuclear Materials Datasheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lan89471\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qci88181\Documents\Outreach\EEW\eew-nuclear\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22380" windowHeight="9285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="5546"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>U235</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>mass</t>
-  </si>
-  <si>
-    <t>C12 density assumes in graphite form</t>
   </si>
   <si>
     <t>low density as gas</t>
@@ -415,21 +412,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.15234375" customWidth="1"/>
+    <col min="2" max="2" width="16.3828125" customWidth="1"/>
+    <col min="3" max="3" width="8.3828125" customWidth="1"/>
+    <col min="12" max="12" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -452,10 +449,10 @@
         <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -479,7 +476,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -493,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E14" si="0">B3+C3+D3</f>
+        <f t="shared" ref="E3:E13" si="0">B3+C3+D3</f>
         <v>13</v>
       </c>
       <c r="F3">
@@ -503,7 +500,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -527,7 +524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -551,7 +548,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -575,10 +572,10 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -602,10 +599,10 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -629,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -656,7 +653,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -680,7 +677,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -704,124 +701,97 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>4.9000000000000004</v>
+        <v>5.08</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>5.08</v>
       </c>
       <c r="F12" s="1">
-        <v>2.2669999999999999</v>
+        <v>2.34</v>
       </c>
       <c r="G12">
-        <v>12</v>
-      </c>
-      <c r="I12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3798</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3800</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.17</v>
+      </c>
+      <c r="G13">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>5.08</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>5.08</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2.34</v>
-      </c>
-      <c r="G13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
+        <v>3.1</v>
+      </c>
+      <c r="D14">
+        <v>0.4</v>
+      </c>
+      <c r="E14">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
         <v>2</v>
       </c>
-      <c r="D14">
-        <v>3798</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>3800</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2.17</v>
-      </c>
-      <c r="G14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>3.1</v>
-      </c>
       <c r="D15">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E15">
-        <v>3.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F15" s="1">
-        <v>8.6999999999999993</v>
+        <v>2.3290000000000002</v>
       </c>
       <c r="G15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>0.2</v>
-      </c>
-      <c r="E16">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2.3290000000000002</v>
-      </c>
-      <c r="G16">
         <v>28</v>
       </c>
     </row>

</xml_diff>